<commit_message>
unit one hundred two - intermediate
</commit_message>
<xml_diff>
--- a/homework/101.xlsx
+++ b/homework/101.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="1386" documentId="13_ncr:1_{6397D056-7233-42F8-9329-AC4D59D3BBF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5C60AA82-D106-47E6-88FB-143D0E51BFF3}"/>
+  <xr:revisionPtr revIDLastSave="1391" documentId="13_ncr:1_{6397D056-7233-42F8-9329-AC4D59D3BBF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{45C760FC-12B9-421F-9FEB-66A2CB119E57}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="1485" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4035" yWindow="1830" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,22 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
-    <t>100.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100.4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>good</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -140,6 +124,22 @@
   </si>
   <si>
     <t>hardly anywhere(any)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101.2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -563,7 +563,7 @@
   <dimension ref="A3:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -578,7 +578,7 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <v>100.1</v>
+        <v>101.1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
@@ -586,7 +586,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
@@ -594,7 +594,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
@@ -602,7 +602,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
@@ -610,7 +610,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
@@ -618,7 +618,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -626,7 +626,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
@@ -634,7 +634,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
@@ -642,7 +642,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
@@ -650,7 +650,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B13" s="5"/>
     </row>
@@ -659,7 +659,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
@@ -667,7 +667,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
@@ -675,7 +675,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
@@ -683,7 +683,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
@@ -691,7 +691,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
@@ -700,7 +700,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -708,7 +708,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B21" s="5"/>
     </row>
@@ -717,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
@@ -725,7 +725,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
@@ -733,7 +733,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
@@ -742,7 +742,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
@@ -750,7 +750,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
@@ -758,7 +758,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B28" s="5"/>
     </row>
@@ -767,7 +767,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
@@ -775,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
@@ -784,7 +784,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
@@ -792,7 +792,7 @@
         <v>5</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
@@ -800,7 +800,7 @@
         <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
@@ -808,7 +808,7 @@
         <v>7</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
@@ -816,7 +816,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B36" s="5"/>
     </row>
@@ -825,7 +825,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
@@ -833,7 +833,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
@@ -841,7 +841,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
@@ -849,7 +849,7 @@
         <v>5</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
@@ -857,7 +857,7 @@
         <v>6</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
@@ -865,7 +865,7 @@
         <v>7</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
@@ -873,7 +873,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
@@ -881,7 +881,7 @@
         <v>9</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
@@ -889,7 +889,7 @@
         <v>10</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>